<commit_message>
solver works with <= in reaction equations
</commit_message>
<xml_diff>
--- a/excel files/propionate_production.xlsx
+++ b/excel files/propionate_production.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1444C188-68C9-4A70-AB2A-0FF1DB09FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3FF3E9-6A20-454F-8DB4-EA529BB69C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>composition</t>
   </si>
   <si>
-    <t>mix_culture</t>
-  </si>
-  <si>
     <t>glu</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>glu, casine, pH</t>
   </si>
   <si>
-    <t>ace == glu*0.0021470197960763663+pH*0.010062441241181396+ 0.2*casine , prop == glu*0.0008586272965669681+pH*0.00128523604994718+0.2*casine, but == glu*0.00343240244820466+pH*-0.007526404480666873 + 0.02*casine</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -279,6 +273,12 @@
   </si>
   <si>
     <t>Propionate, Acetate</t>
+  </si>
+  <si>
+    <t>open_fermentation</t>
+  </si>
+  <si>
+    <t>ace &lt;= glu*0.00213+pH*0.001+ 0.0002*casine , prop &lt;= glu*0.0008+pH*0.00012+0.0002*casine, but &lt;= glu*0.00343+pH*-0.007526 + 0.0002*casine</t>
   </si>
 </sst>
 </file>
@@ -466,15 +466,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:colOff>745490</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>767080</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -489,8 +489,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7734300" y="1809750"/>
-          <a:ext cx="2298700" cy="1587500"/>
+          <a:off x="7609840" y="1809750"/>
+          <a:ext cx="2244090" cy="1790700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1390,22 +1390,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1416,22 +1416,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3">
-        <v>0.8</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1442,13 +1442,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1457,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1468,22 +1468,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1500,16 +1500,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1517,7 +1517,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E13:G13 E2:F2 E3 E4:F9 H2:H9">
+  <conditionalFormatting sqref="E13:G13 E2:F2 H2:H9 E4:F9 E3">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -1532,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2DC50F-7E38-4E45-9660-C41E1DA6142A}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,28 +1558,28 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1591,7 +1591,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1602,25 +1602,25 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="6">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>100</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="6">
         <v>2</v>
@@ -1643,25 +1643,25 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="6">
         <v>0</v>
@@ -1670,7 +1670,7 @@
         <v>100</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="6">
         <v>2</v>
@@ -1684,25 +1684,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="6">
         <v>1</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="6">
         <v>0</v>
@@ -1711,7 +1711,7 @@
         <v>100</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" s="6">
         <v>2</v>
@@ -1725,25 +1725,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="6">
         <v>0</v>
@@ -1752,7 +1752,7 @@
         <v>100</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="6">
         <v>2</v>
@@ -1760,31 +1760,31 @@
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="6">
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="6">
         <v>0</v>
@@ -1793,7 +1793,7 @@
         <v>100</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
@@ -1801,31 +1801,31 @@
     </row>
     <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" s="6">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>100</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="6">
         <v>2</v>
@@ -1857,7 +1857,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1871,140 +1871,140 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="G2" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="G3" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="G4" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="G5" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>78</v>
-      </c>
       <c r="D6" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="G6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,7 +2030,7 @@
     <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="13" max="13" width="8.77734375" customWidth="1"/>
   </cols>
@@ -2040,10 +2040,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -2058,24 +2058,24 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>27</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -2084,22 +2084,22 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -2178,10 +2178,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
@@ -2216,10 +2216,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -2254,10 +2254,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -2292,10 +2292,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -2330,10 +2330,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L8" s="1">
         <v>0</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2368,18 +2368,18 @@
         <v>0</v>
       </c>
       <c r="J9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="L9" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -2541,31 +2541,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -2581,26 +2581,26 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change bool activation, works
</commit_message>
<xml_diff>
--- a/excel files/propionate_production.xlsx
+++ b/excel files/propionate_production.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3FF3E9-6A20-454F-8DB4-EA529BB69C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D0587E-5892-426E-AA37-603E623F6FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -278,7 +278,7 @@
     <t>open_fermentation</t>
   </si>
   <si>
-    <t>ace &lt;= glu*0.00213+pH*0.001+ 0.0002*casine , prop &lt;= glu*0.0008+pH*0.00012+0.0002*casine, but &lt;= glu*0.00343+pH*-0.007526 + 0.0002*casine</t>
+    <t>ace == glu*0.00213+pH*0.001+ 0.0002*casine , prop == glu*0.0008+pH*0.00012+0.0002*casine, but == glu*0.00343+pH*-0.007526 + 0.0002*casine</t>
   </si>
 </sst>
 </file>
@@ -1036,6 +1036,80 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>334010</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3399C56-86A3-37A8-2F0D-7A664D3C5FEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2710180"/>
+          <a:ext cx="10316210" cy="6586220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1340,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1532,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2DC50F-7E38-4E45-9660-C41E1DA6142A}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2016,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2534,7 +2608,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
working by reading in models
</commit_message>
<xml_diff>
--- a/excel files/propionate_production.xlsx
+++ b/excel files/propionate_production.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D0587E-5892-426E-AA37-603E623F6FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D411AD5-E005-48FB-921F-8E2AAD9F6D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
     <sheet name="reactor_intervals" sheetId="2" r:id="rId2"/>
-    <sheet name="sbml_models" sheetId="14" r:id="rId3"/>
+    <sheet name="models" sheetId="14" r:id="rId3"/>
     <sheet name="connection_matrix" sheetId="11" r:id="rId4"/>
     <sheet name="abbr" sheetId="15" r:id="rId5"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
   <si>
     <t>components</t>
   </si>
@@ -278,7 +278,19 @@
     <t>open_fermentation</t>
   </si>
   <si>
-    <t>ace == glu*0.00213+pH*0.001+ 0.0002*casine , prop == glu*0.0008+pH*0.00012+0.0002*casine, but == glu*0.00343+pH*-0.007526 + 0.0002*casine</t>
+    <t>Glucose_open_fermentation.json</t>
+  </si>
+  <si>
+    <t>Propionate, Acetate, Butyrate</t>
+  </si>
+  <si>
+    <t>prop, ace, but</t>
+  </si>
+  <si>
+    <t>Glucose, pH</t>
+  </si>
+  <si>
+    <t>glu,pH</t>
   </si>
 </sst>
 </file>
@@ -1607,7 +1619,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1619,7 +1631,7 @@
     <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.21875" customWidth="1"/>
     <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
@@ -1928,19 +1940,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8D8FB7-0FD2-42C3-9D82-0A6D9AE32488}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2079,6 +2092,29 @@
       </c>
       <c r="G6" s="16" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>